<commit_message>
This update is to include parameterisation through maven parameters
</commit_message>
<xml_diff>
--- a/Framework/TestData/Data.xlsx
+++ b/Framework/TestData/Data.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchahal\eclipse-workspace\Framework\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2C0CD9-40AB-4113-90AB-F9313C4A5068}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{45F87AB7-73EF-48F9-BAB7-D55C0F4FF910}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>